<commit_message>
added some many ideas and sub-projects
</commit_message>
<xml_diff>
--- a/atmega_midi_x0x_heart_own/x0x heart midi device thing part list.xlsx
+++ b/atmega_midi_x0x_heart_own/x0x heart midi device thing part list.xlsx
@@ -622,11 +622,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,7 +638,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,8 +721,8 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -734,7 +734,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -759,82 +759,82 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="3" t="n">
         <v>220</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="3" t="n">
         <v>220</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="3" t="n">
         <v>270</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="3" t="n">
         <v>470</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -842,7 +842,7 @@
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -859,522 +859,522 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1419,142 +1419,142 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1579,142 +1579,142 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>